<commit_message>
add image to dethiso5.xlsx
</commit_message>
<xml_diff>
--- a/dethiso 5.xlsx
+++ b/dethiso 5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\chung chi tin hoc ung dung\Tin hoc CNTTCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chtie\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -293,6 +293,44 @@
         <a:xfrm>
           <a:off x="9029699" y="2124074"/>
           <a:ext cx="1857375" cy="1857375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>332898</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>66048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3629025" y="2314574"/>
+          <a:ext cx="6266973" cy="3533149"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -570,7 +608,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>